<commit_message>
testing if all up to date
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017.xlsx
+++ b/data/TablesZhangetal2017.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forestation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A54EF7D5-C5C6-48E7-956A-ADC6280DEAF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA21B078-3147-4962-BC41-DB0091A7B26D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="531">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1669,6 +1669,12 @@
   </si>
   <si>
     <t>Yerrami.  S</t>
+  </si>
+  <si>
+    <t>Latititude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1780,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1786,7 +1789,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2112,54 +2118,54 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -3413,7 +3419,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -4304,100 +4310,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
-  <dimension ref="A1:K253"/>
+  <dimension ref="A1:M253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A228" sqref="A228:K253"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" t="s">
+        <v>529</v>
+      </c>
+      <c r="M2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>62</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C3" s="4">
         <v>3.03</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="8">
         <v>2474</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="8">
         <v>-25</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="8">
         <v>7.9</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>63</v>
       </c>
@@ -4432,7 +4444,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>64</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>65</v>
       </c>
@@ -4502,7 +4514,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>66</v>
       </c>
@@ -4537,7 +4549,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>67</v>
       </c>
@@ -4572,7 +4584,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>68</v>
       </c>
@@ -4607,7 +4619,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>69</v>
       </c>
@@ -4642,7 +4654,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>70</v>
       </c>
@@ -4677,7 +4689,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>71</v>
       </c>
@@ -4712,7 +4724,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>72</v>
       </c>
@@ -4747,7 +4759,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>73</v>
       </c>
@@ -4782,7 +4794,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>74</v>
       </c>
@@ -4817,7 +4829,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>75</v>
       </c>
@@ -5762,7 +5774,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>102</v>
       </c>
@@ -6602,7 +6614,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>126</v>
       </c>
@@ -7547,7 +7559,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>153</v>
       </c>
@@ -8562,7 +8574,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>182</v>
       </c>
@@ -9542,7 +9554,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>210</v>
       </c>
@@ -10487,7 +10499,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A178" s="4">
         <v>237</v>
       </c>
@@ -11432,7 +11444,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A205" s="4">
         <v>290</v>
       </c>
@@ -12238,37 +12250,37 @@
       </c>
     </row>
     <row r="228" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A228" s="12">
+      <c r="A228" s="8">
         <v>257</v>
       </c>
-      <c r="B228" s="12" t="s">
+      <c r="B228" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="C228" s="12">
+      <c r="C228" s="8">
         <v>130</v>
       </c>
-      <c r="D228" s="12">
+      <c r="D228" s="8">
         <v>707</v>
       </c>
-      <c r="E228" s="12" t="s">
+      <c r="E228" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F228" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G228" s="12">
+      <c r="F228" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G228" s="8">
         <v>-40</v>
       </c>
-      <c r="H228" s="12">
+      <c r="H228" s="8">
         <v>0</v>
       </c>
-      <c r="I228" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J228" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K228" s="12" t="s">
+      <c r="I228" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J228" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K228" s="8" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
collecting new data Zhang et al. 2011
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017.xlsx
+++ b/data/TablesZhangetal2017.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA21B078-3147-4962-BC41-DB0091A7B26D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02996C0-CBB3-4F7C-A074-A2CE12C65917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
     <sheet name="Zhang et al. (2017) &lt; 1000 km2" sheetId="2" r:id="rId2"/>
+    <sheet name="NewData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="549">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1675,6 +1676,60 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Adjungbilly Creek</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>Battaling Ck</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>Zhang et al. 2011</t>
+  </si>
+  <si>
+    <t>Bombala River</t>
+  </si>
+  <si>
+    <t>Burnt Out Ck</t>
+  </si>
+  <si>
+    <t>Crawford River</t>
+  </si>
+  <si>
+    <t>Darlot Ck</t>
+  </si>
+  <si>
+    <t>Delegate River</t>
+  </si>
+  <si>
+    <t>Eumeralla River</t>
+  </si>
+  <si>
+    <t>Goobarragandra Ck</t>
+  </si>
+  <si>
+    <t>Jingellic Ck</t>
+  </si>
+  <si>
+    <t>Pine Ck</t>
+  </si>
+  <si>
+    <t>Traralgon Ck</t>
+  </si>
+  <si>
+    <t>Upper Denmark River</t>
+  </si>
+  <si>
+    <t>Yate Flat Ck</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1781,6 +1836,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2118,54 +2176,54 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -4312,61 +4370,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:M253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="L2" t="s">
         <v>529</v>
       </c>
@@ -13157,6 +13215,757 @@
       </c>
       <c r="K253" s="6" t="s">
         <v>483</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" t="s">
+        <v>529</v>
+      </c>
+      <c r="M2" t="s">
+        <v>530</v>
+      </c>
+      <c r="N2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>283</v>
+      </c>
+      <c r="B3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C3">
+        <v>391</v>
+      </c>
+      <c r="D3">
+        <v>1011</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>535</v>
+      </c>
+      <c r="G3">
+        <v>30.08</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>536</v>
+      </c>
+      <c r="L3">
+        <v>-32.020000000000003</v>
+      </c>
+      <c r="M3">
+        <v>148.25</v>
+      </c>
+      <c r="N3">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>284</v>
+      </c>
+      <c r="B4" t="s">
+        <v>534</v>
+      </c>
+      <c r="C4">
+        <v>16.64</v>
+      </c>
+      <c r="D4">
+        <v>629</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>533</v>
+      </c>
+      <c r="G4">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>536</v>
+      </c>
+      <c r="L4">
+        <v>-33.32</v>
+      </c>
+      <c r="M4">
+        <v>116.57</v>
+      </c>
+      <c r="N4">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>537</v>
+      </c>
+      <c r="C5">
+        <v>559</v>
+      </c>
+      <c r="D5">
+        <v>783</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>535</v>
+      </c>
+      <c r="G5">
+        <v>26.8</v>
+      </c>
+      <c r="H5">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>536</v>
+      </c>
+      <c r="L5">
+        <v>-37</v>
+      </c>
+      <c r="M5">
+        <v>149.38</v>
+      </c>
+      <c r="N5">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>286</v>
+      </c>
+      <c r="B6" t="s">
+        <v>538</v>
+      </c>
+      <c r="C6">
+        <v>0.6</v>
+      </c>
+      <c r="D6">
+        <v>806</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>533</v>
+      </c>
+      <c r="G6">
+        <v>67</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>536</v>
+      </c>
+      <c r="L6">
+        <v>-35.130000000000003</v>
+      </c>
+      <c r="M6">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="N6">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>287</v>
+      </c>
+      <c r="B7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C7">
+        <v>606</v>
+      </c>
+      <c r="D7">
+        <v>728</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>533</v>
+      </c>
+      <c r="G7">
+        <v>24.18</v>
+      </c>
+      <c r="H7">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>536</v>
+      </c>
+      <c r="L7">
+        <v>-37.979999999999997</v>
+      </c>
+      <c r="M7">
+        <v>141.46</v>
+      </c>
+      <c r="N7">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>288</v>
+      </c>
+      <c r="B8" t="s">
+        <v>540</v>
+      </c>
+      <c r="C8">
+        <v>760</v>
+      </c>
+      <c r="D8">
+        <v>688</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>533</v>
+      </c>
+      <c r="G8">
+        <v>13.3</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>536</v>
+      </c>
+      <c r="L8">
+        <v>-38.15</v>
+      </c>
+      <c r="M8">
+        <v>141.77000000000001</v>
+      </c>
+      <c r="N8">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>289</v>
+      </c>
+      <c r="B9" t="s">
+        <v>541</v>
+      </c>
+      <c r="C9">
+        <v>1135.7</v>
+      </c>
+      <c r="D9">
+        <v>859</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>535</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>536</v>
+      </c>
+      <c r="L9">
+        <v>-36.979999999999997</v>
+      </c>
+      <c r="M9">
+        <v>149.05000000000001</v>
+      </c>
+      <c r="N9">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>290</v>
+      </c>
+      <c r="B10" t="s">
+        <v>542</v>
+      </c>
+      <c r="C10">
+        <v>502</v>
+      </c>
+      <c r="D10">
+        <v>725</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>533</v>
+      </c>
+      <c r="G10">
+        <v>19.84</v>
+      </c>
+      <c r="H10">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>536</v>
+      </c>
+      <c r="L10">
+        <v>-38.26</v>
+      </c>
+      <c r="M10">
+        <v>141.94</v>
+      </c>
+      <c r="N10">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>291</v>
+      </c>
+      <c r="B11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C11">
+        <v>673</v>
+      </c>
+      <c r="D11">
+        <v>1009</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>535</v>
+      </c>
+      <c r="G11">
+        <v>8.32</v>
+      </c>
+      <c r="H11">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>536</v>
+      </c>
+      <c r="L11">
+        <v>-35.19</v>
+      </c>
+      <c r="M11">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="N11">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>292</v>
+      </c>
+      <c r="B12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C12">
+        <v>390</v>
+      </c>
+      <c r="D12">
+        <v>838</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>535</v>
+      </c>
+      <c r="G12">
+        <v>27.5</v>
+      </c>
+      <c r="H12">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>536</v>
+      </c>
+      <c r="L12">
+        <v>-35.53</v>
+      </c>
+      <c r="M12">
+        <v>147.41</v>
+      </c>
+      <c r="N12">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>293</v>
+      </c>
+      <c r="B13" t="s">
+        <v>545</v>
+      </c>
+      <c r="C13">
+        <v>3.2</v>
+      </c>
+      <c r="D13">
+        <v>629</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>533</v>
+      </c>
+      <c r="G13">
+        <v>88</v>
+      </c>
+      <c r="H13">
+        <v>106</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>536</v>
+      </c>
+      <c r="L13">
+        <v>-37.29</v>
+      </c>
+      <c r="M13">
+        <v>145.05000000000001</v>
+      </c>
+      <c r="N13">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>294</v>
+      </c>
+      <c r="B14" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14">
+        <v>1.95</v>
+      </c>
+      <c r="D14">
+        <v>760</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>533</v>
+      </c>
+      <c r="G14">
+        <v>78</v>
+      </c>
+      <c r="H14">
+        <v>66</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" t="s">
+        <v>536</v>
+      </c>
+      <c r="L14">
+        <v>-35.119999999999997</v>
+      </c>
+      <c r="M14">
+        <v>149.35</v>
+      </c>
+      <c r="N14">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>295</v>
+      </c>
+      <c r="B15" t="s">
+        <v>546</v>
+      </c>
+      <c r="C15">
+        <v>89</v>
+      </c>
+      <c r="D15">
+        <v>959</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>535</v>
+      </c>
+      <c r="G15">
+        <v>58</v>
+      </c>
+      <c r="H15">
+        <v>78</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>536</v>
+      </c>
+      <c r="L15">
+        <v>-38.32</v>
+      </c>
+      <c r="M15">
+        <v>146.53</v>
+      </c>
+      <c r="N15">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>296</v>
+      </c>
+      <c r="B16" t="s">
+        <v>547</v>
+      </c>
+      <c r="C16">
+        <v>243</v>
+      </c>
+      <c r="D16">
+        <v>742</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>535</v>
+      </c>
+      <c r="G16">
+        <v>15.17</v>
+      </c>
+      <c r="H16">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
+        <v>536</v>
+      </c>
+      <c r="L16">
+        <v>-34.700000000000003</v>
+      </c>
+      <c r="M16">
+        <v>117.22</v>
+      </c>
+      <c r="N16">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>297</v>
+      </c>
+      <c r="B17" t="s">
+        <v>548</v>
+      </c>
+      <c r="C17">
+        <v>26.35</v>
+      </c>
+      <c r="D17">
+        <v>742</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>535</v>
+      </c>
+      <c r="G17">
+        <v>33.57</v>
+      </c>
+      <c r="H17">
+        <v>91</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
+        <v>536</v>
+      </c>
+      <c r="L17">
+        <v>-33.700000000000003</v>
+      </c>
+      <c r="M17">
+        <v>117.29</v>
+      </c>
+      <c r="N17">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Borg et al. 1988
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017.xlsx
+++ b/data/TablesZhangetal2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02996C0-CBB3-4F7C-A074-A2CE12C65917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A485BB41-39CD-4431-9AEC-454E36EE4070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="2064" yWindow="348" windowWidth="19404" windowHeight="11400" activeTab="2" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="551">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1730,6 +1730,12 @@
   </si>
   <si>
     <t>Yate Flat Ck</t>
+  </si>
+  <si>
+    <t>Borg et al. 1988</t>
+  </si>
+  <si>
+    <t>Padbury reservoir catchment</t>
   </si>
 </sst>
 </file>
@@ -4370,7 +4376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:M253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A178" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
@@ -13239,7 +13245,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13326,7 +13332,7 @@
         <v>30.08</v>
       </c>
       <c r="H3">
-        <v>60</v>
+        <v>-60</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
@@ -13370,7 +13376,7 @@
         <v>19</v>
       </c>
       <c r="H4">
-        <v>52</v>
+        <v>-52</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
@@ -13414,7 +13420,7 @@
         <v>26.8</v>
       </c>
       <c r="H5">
-        <v>29</v>
+        <v>-29</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -13458,7 +13464,7 @@
         <v>67</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
@@ -13502,7 +13508,7 @@
         <v>24.18</v>
       </c>
       <c r="H7">
-        <v>66</v>
+        <v>-66</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
@@ -13546,7 +13552,7 @@
         <v>13.3</v>
       </c>
       <c r="H8">
-        <v>28</v>
+        <v>-28</v>
       </c>
       <c r="I8" t="s">
         <v>15</v>
@@ -13590,7 +13596,7 @@
         <v>14</v>
       </c>
       <c r="H9">
-        <v>52</v>
+        <v>-52</v>
       </c>
       <c r="I9" t="s">
         <v>15</v>
@@ -13634,7 +13640,7 @@
         <v>19.84</v>
       </c>
       <c r="H10">
-        <v>57</v>
+        <v>-57</v>
       </c>
       <c r="I10" t="s">
         <v>15</v>
@@ -13678,7 +13684,7 @@
         <v>8.32</v>
       </c>
       <c r="H11">
-        <v>35</v>
+        <v>-35</v>
       </c>
       <c r="I11" t="s">
         <v>15</v>
@@ -13722,7 +13728,7 @@
         <v>27.5</v>
       </c>
       <c r="H12">
-        <v>37</v>
+        <v>-37</v>
       </c>
       <c r="I12" t="s">
         <v>15</v>
@@ -13766,7 +13772,7 @@
         <v>88</v>
       </c>
       <c r="H13">
-        <v>106</v>
+        <v>-106</v>
       </c>
       <c r="I13" t="s">
         <v>15</v>
@@ -13810,7 +13816,7 @@
         <v>78</v>
       </c>
       <c r="H14">
-        <v>66</v>
+        <v>-66</v>
       </c>
       <c r="I14" t="s">
         <v>15</v>
@@ -13854,7 +13860,7 @@
         <v>58</v>
       </c>
       <c r="H15">
-        <v>78</v>
+        <v>-78</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -13898,7 +13904,7 @@
         <v>15.17</v>
       </c>
       <c r="H16">
-        <v>93</v>
+        <v>-93</v>
       </c>
       <c r="I16" t="s">
         <v>15</v>
@@ -13942,7 +13948,7 @@
         <v>33.57</v>
       </c>
       <c r="H17">
-        <v>91</v>
+        <v>-91</v>
       </c>
       <c r="I17" t="s">
         <v>15</v>
@@ -13966,6 +13972,43 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>298</v>
+      </c>
+      <c r="B18" t="s">
+        <v>550</v>
+      </c>
+      <c r="C18">
+        <f>196.4/100</f>
+        <v>1.964</v>
+      </c>
+      <c r="D18">
+        <v>880</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>533</v>
+      </c>
+      <c r="G18">
+        <v>60.9</v>
+      </c>
+      <c r="H18">
+        <v>-92</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" t="s">
+        <v>549</v>
+      </c>
+      <c r="L18">
+        <v>-33.810141399699802</v>
+      </c>
+      <c r="M18">
+        <v>116.003923121299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further paper updates and data correction
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017.xlsx
+++ b/data/TablesZhangetal2017.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanin\Documents\GitHub\Forest_and_water\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CEC6C6-BB9B-43E0-9D6E-B9868C7609FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C9E234-0A2D-464C-8F71-C9438C7790A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
     <sheet name="Zhang et al. (2017) &lt; 1000 km2" sheetId="2" r:id="rId2"/>
     <sheet name="NewData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2463,6 +2472,12 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2473,12 +2488,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2797,24 +2806,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CA6CB8-28F4-480A-8011-F310B3E1710B}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="8.7265625" style="17"/>
-    <col min="11" max="11" width="17.81640625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.36328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.90625" style="18" customWidth="1"/>
-    <col min="15" max="15" width="18.90625" style="20" customWidth="1"/>
-    <col min="16" max="16" width="65.453125" style="17" customWidth="1"/>
-    <col min="17" max="17" width="9.7265625" style="17" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="17"/>
+    <col min="1" max="10" width="8.77734375" style="17"/>
+    <col min="11" max="11" width="17.77734375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" style="20" customWidth="1"/>
+    <col min="16" max="16" width="65.44140625" style="17" customWidth="1"/>
+    <col min="17" max="17" width="9.77734375" style="17" customWidth="1"/>
+    <col min="18" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="142.80000000000001" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2916,11 +2925,11 @@
       <c r="P2" s="18" t="s">
         <v>607</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="18" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="101.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3129,7 +3138,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3179,7 +3188,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3229,7 +3238,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3279,7 +3288,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3332,7 +3341,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3382,7 +3391,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3535,7 +3544,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3635,7 +3644,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3688,7 +3697,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3788,7 +3797,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3838,7 +3847,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3888,7 +3897,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3991,7 +4000,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -4044,7 +4053,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -4097,7 +4106,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -4150,7 +4159,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -4248,7 +4257,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="29.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -4296,7 +4305,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -4346,7 +4355,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="58.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -4396,7 +4405,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="58.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="292.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="292.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -4499,7 +4508,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -4549,7 +4558,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -4594,7 +4603,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -4639,7 +4648,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -4689,7 +4698,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -4736,7 +4745,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -4786,7 +4795,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -4833,7 +4842,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -4883,7 +4892,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -4933,7 +4942,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -4983,7 +4992,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="72.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="72.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -5033,7 +5042,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5083,7 +5092,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -5133,7 +5142,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -5186,7 +5195,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="58.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -5236,7 +5245,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -5289,7 +5298,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -5339,7 +5348,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -5392,7 +5401,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="116" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="115.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -5445,7 +5454,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -5495,7 +5504,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -5540,7 +5549,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -5590,7 +5599,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -5640,7 +5649,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -5690,7 +5699,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -5738,7 +5747,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" ht="28.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -5788,7 +5797,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -5835,7 +5844,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -5885,7 +5894,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="218" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="217.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5952,19 +5961,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:S252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+    <sheetView topLeftCell="C64" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1796875" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -5983,10 +5992,10 @@
       <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="24" t="s">
@@ -6023,7 +6032,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>62</v>
       </c>
@@ -6074,7 +6083,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>63</v>
       </c>
@@ -6125,7 +6134,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>64</v>
       </c>
@@ -6175,7 +6184,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>65</v>
       </c>
@@ -6226,7 +6235,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>66</v>
       </c>
@@ -6274,7 +6283,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>67</v>
       </c>
@@ -6324,7 +6333,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>68</v>
       </c>
@@ -6369,7 +6378,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>69</v>
       </c>
@@ -6405,7 +6414,7 @@
       </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>70</v>
       </c>
@@ -6441,7 +6450,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>71</v>
       </c>
@@ -6477,7 +6486,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>72</v>
       </c>
@@ -6516,7 +6525,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>73</v>
       </c>
@@ -6557,7 +6566,7 @@
       <c r="N13">
         <v>64.066666999999995</v>
       </c>
-      <c r="O13" s="30"/>
+      <c r="O13" s="26"/>
       <c r="P13" t="s">
         <v>718</v>
       </c>
@@ -6571,7 +6580,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>74</v>
       </c>
@@ -6607,7 +6616,7 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>75</v>
       </c>
@@ -6643,7 +6652,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>76</v>
       </c>
@@ -6684,7 +6693,7 @@
       <c r="N16">
         <v>-111.667858</v>
       </c>
-      <c r="O16" s="30"/>
+      <c r="O16" s="26"/>
       <c r="P16" t="s">
         <v>716</v>
       </c>
@@ -6698,7 +6707,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>77</v>
       </c>
@@ -6737,7 +6746,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>78</v>
       </c>
@@ -6773,7 +6782,7 @@
       </c>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>79</v>
       </c>
@@ -6809,7 +6818,7 @@
       </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>80</v>
       </c>
@@ -6845,7 +6854,7 @@
       </c>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>81</v>
       </c>
@@ -6881,7 +6890,7 @@
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>82</v>
       </c>
@@ -6917,7 +6926,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>83</v>
       </c>
@@ -6956,7 +6965,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>84</v>
       </c>
@@ -6992,7 +7001,7 @@
       </c>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>85</v>
       </c>
@@ -7028,7 +7037,7 @@
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>86</v>
       </c>
@@ -7064,7 +7073,7 @@
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>87</v>
       </c>
@@ -7100,7 +7109,7 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>88</v>
       </c>
@@ -7136,7 +7145,7 @@
       </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>89</v>
       </c>
@@ -7177,7 +7186,7 @@
       <c r="N29">
         <v>65.150000000000006</v>
       </c>
-      <c r="O29" s="30"/>
+      <c r="O29" s="26"/>
       <c r="P29" t="s">
         <v>719</v>
       </c>
@@ -7185,7 +7194,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>90</v>
       </c>
@@ -7226,7 +7235,7 @@
       <c r="N30">
         <v>122.833333</v>
       </c>
-      <c r="O30" s="30"/>
+      <c r="O30" s="26"/>
       <c r="Q30">
         <v>1980</v>
       </c>
@@ -7237,7 +7246,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>91</v>
       </c>
@@ -7273,7 +7282,7 @@
       </c>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>92</v>
       </c>
@@ -7309,7 +7318,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>93</v>
       </c>
@@ -7345,7 +7354,7 @@
       </c>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>94</v>
       </c>
@@ -7381,7 +7390,7 @@
       </c>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>95</v>
       </c>
@@ -7417,7 +7426,7 @@
       </c>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>96</v>
       </c>
@@ -7453,7 +7462,7 @@
       </c>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>97</v>
       </c>
@@ -7494,7 +7503,7 @@
       <c r="N37">
         <v>65.116667000000007</v>
       </c>
-      <c r="O37" s="30"/>
+      <c r="O37" s="26"/>
       <c r="P37" t="s">
         <v>720</v>
       </c>
@@ -7502,7 +7511,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>98</v>
       </c>
@@ -7538,7 +7547,7 @@
       </c>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>99</v>
       </c>
@@ -7574,7 +7583,7 @@
       </c>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>100</v>
       </c>
@@ -7613,7 +7622,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>101</v>
       </c>
@@ -7649,7 +7658,7 @@
       </c>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>102</v>
       </c>
@@ -7693,7 +7702,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>103</v>
       </c>
@@ -7729,7 +7738,7 @@
       </c>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>104</v>
       </c>
@@ -7765,7 +7774,7 @@
       </c>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>105</v>
       </c>
@@ -7801,7 +7810,7 @@
       </c>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>106</v>
       </c>
@@ -7837,7 +7846,7 @@
       </c>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>107</v>
       </c>
@@ -7873,7 +7882,7 @@
       </c>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>108</v>
       </c>
@@ -7909,7 +7918,7 @@
       </c>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>109</v>
       </c>
@@ -7945,7 +7954,7 @@
       </c>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>110</v>
       </c>
@@ -7981,7 +7990,7 @@
       </c>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>111</v>
       </c>
@@ -8017,7 +8026,7 @@
       </c>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:19" ht="50" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>112</v>
       </c>
@@ -8053,7 +8062,7 @@
       </c>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>113</v>
       </c>
@@ -8089,7 +8098,7 @@
       </c>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>114</v>
       </c>
@@ -8125,7 +8134,7 @@
       </c>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>115</v>
       </c>
@@ -8161,7 +8170,7 @@
       </c>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>116</v>
       </c>
@@ -8197,7 +8206,7 @@
       </c>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>117</v>
       </c>
@@ -8233,7 +8242,7 @@
       </c>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>118</v>
       </c>
@@ -8269,7 +8278,7 @@
       </c>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>119</v>
       </c>
@@ -8305,7 +8314,7 @@
       </c>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>120</v>
       </c>
@@ -8341,7 +8350,7 @@
       </c>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>121</v>
       </c>
@@ -8377,7 +8386,7 @@
       </c>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>122</v>
       </c>
@@ -8413,7 +8422,7 @@
       </c>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>123</v>
       </c>
@@ -8454,7 +8463,7 @@
       <c r="N63">
         <v>64.05</v>
       </c>
-      <c r="O63" s="30"/>
+      <c r="O63" s="26"/>
       <c r="P63" t="s">
         <v>721</v>
       </c>
@@ -8462,7 +8471,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>124</v>
       </c>
@@ -8503,7 +8512,7 @@
       <c r="N64">
         <v>76.7</v>
       </c>
-      <c r="O64" s="30"/>
+      <c r="O64" s="26"/>
       <c r="Q64">
         <v>2002</v>
       </c>
@@ -8514,7 +8523,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>125</v>
       </c>
@@ -8550,7 +8559,7 @@
       </c>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>126</v>
       </c>
@@ -8586,7 +8595,7 @@
       </c>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>127</v>
       </c>
@@ -8622,7 +8631,7 @@
       </c>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>128</v>
       </c>
@@ -8658,7 +8667,7 @@
       </c>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>129</v>
       </c>
@@ -8694,7 +8703,7 @@
       </c>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>130</v>
       </c>
@@ -8730,7 +8739,7 @@
       </c>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>131</v>
       </c>
@@ -8780,7 +8789,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>132</v>
       </c>
@@ -8821,7 +8830,7 @@
       <c r="N72">
         <v>67</v>
       </c>
-      <c r="O72" s="30"/>
+      <c r="O72" s="26"/>
       <c r="P72" t="s">
         <v>722</v>
       </c>
@@ -8829,7 +8838,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="50" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>133</v>
       </c>
@@ -8865,7 +8874,7 @@
       </c>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>134</v>
       </c>
@@ -8901,7 +8910,7 @@
       </c>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>135</v>
       </c>
@@ -8937,7 +8946,7 @@
       </c>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>136</v>
       </c>
@@ -8973,7 +8982,7 @@
       </c>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>137</v>
       </c>
@@ -9009,7 +9018,7 @@
       </c>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>138</v>
       </c>
@@ -9045,7 +9054,7 @@
       </c>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>139</v>
       </c>
@@ -9081,7 +9090,7 @@
       </c>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>140</v>
       </c>
@@ -9117,7 +9126,7 @@
       </c>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>141</v>
       </c>
@@ -9153,7 +9162,7 @@
       </c>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>142</v>
       </c>
@@ -9189,7 +9198,7 @@
       </c>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>143</v>
       </c>
@@ -9225,7 +9234,7 @@
       </c>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4">
         <v>144</v>
       </c>
@@ -9261,7 +9270,7 @@
       </c>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>145</v>
       </c>
@@ -9297,7 +9306,7 @@
       </c>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>146</v>
       </c>
@@ -9333,7 +9342,7 @@
       </c>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>147</v>
       </c>
@@ -9369,7 +9378,7 @@
       </c>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>148</v>
       </c>
@@ -9405,7 +9414,7 @@
       </c>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>149</v>
       </c>
@@ -9441,7 +9450,7 @@
       </c>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>150</v>
       </c>
@@ -9477,7 +9486,7 @@
       </c>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>151</v>
       </c>
@@ -9513,7 +9522,7 @@
       </c>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>152</v>
       </c>
@@ -9549,7 +9558,7 @@
       </c>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>153</v>
       </c>
@@ -9590,7 +9599,7 @@
       <c r="N93">
         <v>-105.881969</v>
       </c>
-      <c r="O93" s="30"/>
+      <c r="O93" s="26"/>
       <c r="P93" t="s">
         <v>714</v>
       </c>
@@ -9604,7 +9613,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>154</v>
       </c>
@@ -9640,7 +9649,7 @@
       </c>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>155</v>
       </c>
@@ -9676,7 +9685,7 @@
       </c>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>156</v>
       </c>
@@ -9717,7 +9726,7 @@
       <c r="N96">
         <v>-105.881742</v>
       </c>
-      <c r="O96" s="30"/>
+      <c r="O96" s="26"/>
       <c r="P96" t="s">
         <v>715</v>
       </c>
@@ -9731,7 +9740,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>157</v>
       </c>
@@ -9772,7 +9781,7 @@
       <c r="N97">
         <v>-105.881742</v>
       </c>
-      <c r="O97" s="30"/>
+      <c r="O97" s="26"/>
       <c r="P97" t="s">
         <v>713</v>
       </c>
@@ -9786,7 +9795,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A98" s="9">
         <v>158</v>
       </c>
@@ -9821,12 +9830,12 @@
         <v>286</v>
       </c>
       <c r="L98" s="2"/>
-      <c r="O98" s="30"/>
+      <c r="O98" s="26"/>
       <c r="P98" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>159</v>
       </c>
@@ -9862,7 +9871,7 @@
       </c>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>160</v>
       </c>
@@ -9898,7 +9907,7 @@
       </c>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>161</v>
       </c>
@@ -9939,7 +9948,7 @@
       <c r="N101">
         <v>66.083332999999996</v>
       </c>
-      <c r="O101" s="30"/>
+      <c r="O101" s="26"/>
       <c r="P101" t="s">
         <v>723</v>
       </c>
@@ -9947,7 +9956,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>162</v>
       </c>
@@ -9988,7 +9997,7 @@
       <c r="N102">
         <v>64.066666999999995</v>
       </c>
-      <c r="O102" s="30"/>
+      <c r="O102" s="26"/>
       <c r="P102" t="s">
         <v>724</v>
       </c>
@@ -9996,7 +10005,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>163</v>
       </c>
@@ -10037,7 +10046,7 @@
       <c r="N103">
         <v>66.016666999999998</v>
       </c>
-      <c r="O103" s="30"/>
+      <c r="O103" s="26"/>
       <c r="P103" t="s">
         <v>725</v>
       </c>
@@ -10045,7 +10054,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>164</v>
       </c>
@@ -10081,7 +10090,7 @@
       </c>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>165</v>
       </c>
@@ -10117,7 +10126,7 @@
       </c>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>166</v>
       </c>
@@ -10153,7 +10162,7 @@
       </c>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>167</v>
       </c>
@@ -10200,7 +10209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>168</v>
       </c>
@@ -10236,7 +10245,7 @@
       </c>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>169</v>
       </c>
@@ -10272,7 +10281,7 @@
       </c>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>170</v>
       </c>
@@ -10308,7 +10317,7 @@
       </c>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>171</v>
       </c>
@@ -10344,7 +10353,7 @@
       </c>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
         <v>172</v>
       </c>
@@ -10380,7 +10389,7 @@
       </c>
       <c r="L112" s="9"/>
     </row>
-    <row r="113" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>173</v>
       </c>
@@ -10416,7 +10425,7 @@
       </c>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>174</v>
       </c>
@@ -10452,7 +10461,7 @@
       </c>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>175</v>
       </c>
@@ -10488,7 +10497,7 @@
       </c>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>176</v>
       </c>
@@ -10524,7 +10533,7 @@
       </c>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>177</v>
       </c>
@@ -10560,7 +10569,7 @@
       </c>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>178</v>
       </c>
@@ -10596,7 +10605,7 @@
       </c>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>179</v>
       </c>
@@ -10632,7 +10641,7 @@
       </c>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>180</v>
       </c>
@@ -10668,7 +10677,7 @@
       </c>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>181</v>
       </c>
@@ -10709,7 +10718,7 @@
       <c r="N121">
         <v>66.083332999999996</v>
       </c>
-      <c r="O121" s="30"/>
+      <c r="O121" s="26"/>
       <c r="P121" t="s">
         <v>726</v>
       </c>
@@ -10717,7 +10726,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>182</v>
       </c>
@@ -10753,7 +10762,7 @@
       </c>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>183</v>
       </c>
@@ -10789,7 +10798,7 @@
       </c>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A124" s="9">
         <v>184</v>
       </c>
@@ -10825,7 +10834,7 @@
       </c>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>185</v>
       </c>
@@ -10861,7 +10870,7 @@
       </c>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>186</v>
       </c>
@@ -10897,7 +10906,7 @@
       </c>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>187</v>
       </c>
@@ -10933,7 +10942,7 @@
       </c>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>188</v>
       </c>
@@ -10969,7 +10978,7 @@
       </c>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="9">
         <v>189</v>
       </c>
@@ -11005,7 +11014,7 @@
       </c>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>190</v>
       </c>
@@ -11041,7 +11050,7 @@
       </c>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>191</v>
       </c>
@@ -11077,7 +11086,7 @@
       </c>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>192</v>
       </c>
@@ -11113,7 +11122,7 @@
       </c>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>193</v>
       </c>
@@ -11149,7 +11158,7 @@
       </c>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>194</v>
       </c>
@@ -11185,7 +11194,7 @@
       </c>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>195</v>
       </c>
@@ -11221,7 +11230,7 @@
       </c>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>196</v>
       </c>
@@ -11257,7 +11266,7 @@
       </c>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>197</v>
       </c>
@@ -11293,7 +11302,7 @@
       </c>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>198</v>
       </c>
@@ -11329,7 +11338,7 @@
       </c>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>199</v>
       </c>
@@ -11370,7 +11379,7 @@
       <c r="N139">
         <v>122.833333</v>
       </c>
-      <c r="O139" s="30"/>
+      <c r="O139" s="26"/>
       <c r="Q139">
         <v>1986</v>
       </c>
@@ -11381,7 +11390,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4">
         <v>200</v>
       </c>
@@ -11417,7 +11426,7 @@
       </c>
       <c r="L140" s="9"/>
     </row>
-    <row r="141" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>201</v>
       </c>
@@ -11453,7 +11462,7 @@
       </c>
       <c r="L141" s="2"/>
     </row>
-    <row r="142" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>202</v>
       </c>
@@ -11489,7 +11498,7 @@
       </c>
       <c r="L142" s="2"/>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>203</v>
       </c>
@@ -11525,7 +11534,7 @@
       </c>
       <c r="L143" s="2"/>
     </row>
-    <row r="144" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>204</v>
       </c>
@@ -11561,7 +11570,7 @@
       </c>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>205</v>
       </c>
@@ -11597,7 +11606,7 @@
       </c>
       <c r="L145" s="2"/>
     </row>
-    <row r="146" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>206</v>
       </c>
@@ -11633,7 +11642,7 @@
       </c>
       <c r="L146" s="2"/>
     </row>
-    <row r="147" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>207</v>
       </c>
@@ -11669,7 +11678,7 @@
       </c>
       <c r="L147" s="2"/>
     </row>
-    <row r="148" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>208</v>
       </c>
@@ -11705,7 +11714,7 @@
       </c>
       <c r="L148" s="2"/>
     </row>
-    <row r="149" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>209</v>
       </c>
@@ -11741,7 +11750,7 @@
       </c>
       <c r="L149" s="2"/>
     </row>
-    <row r="150" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>210</v>
       </c>
@@ -11782,7 +11791,7 @@
       <c r="N150">
         <v>116.32878700000001</v>
       </c>
-      <c r="O150" s="30"/>
+      <c r="O150" s="26"/>
       <c r="Q150">
         <v>1982</v>
       </c>
@@ -11793,7 +11802,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>211</v>
       </c>
@@ -11829,7 +11838,7 @@
       </c>
       <c r="L151" s="2"/>
     </row>
-    <row r="152" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A152" s="9">
         <v>212</v>
       </c>
@@ -11865,7 +11874,7 @@
       </c>
       <c r="L152" s="2"/>
     </row>
-    <row r="153" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>213</v>
       </c>
@@ -11901,7 +11910,7 @@
       </c>
       <c r="L153" s="2"/>
     </row>
-    <row r="154" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>214</v>
       </c>
@@ -11937,7 +11946,7 @@
       </c>
       <c r="L154" s="2"/>
     </row>
-    <row r="155" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A155" s="9">
         <v>215</v>
       </c>
@@ -11973,7 +11982,7 @@
       </c>
       <c r="L155" s="2"/>
     </row>
-    <row r="156" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>216</v>
       </c>
@@ -12009,7 +12018,7 @@
       </c>
       <c r="L156" s="2"/>
     </row>
-    <row r="157" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>217</v>
       </c>
@@ -12045,7 +12054,7 @@
       </c>
       <c r="L157" s="2"/>
     </row>
-    <row r="158" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>218</v>
       </c>
@@ -12081,7 +12090,7 @@
       </c>
       <c r="L158" s="2"/>
     </row>
-    <row r="159" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:19" ht="51" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>219</v>
       </c>
@@ -12117,7 +12126,7 @@
       </c>
       <c r="L159" s="2"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>220</v>
       </c>
@@ -12153,7 +12162,7 @@
       </c>
       <c r="L160" s="2"/>
     </row>
-    <row r="161" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>221</v>
       </c>
@@ -12189,7 +12198,7 @@
       </c>
       <c r="L161" s="2"/>
     </row>
-    <row r="162" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>222</v>
       </c>
@@ -12225,7 +12234,7 @@
       </c>
       <c r="L162" s="2"/>
     </row>
-    <row r="163" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>223</v>
       </c>
@@ -12261,7 +12270,7 @@
       </c>
       <c r="L163" s="2"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="9">
         <v>224</v>
       </c>
@@ -12297,7 +12306,7 @@
       </c>
       <c r="L164" s="2"/>
     </row>
-    <row r="165" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>225</v>
       </c>
@@ -12333,7 +12342,7 @@
       </c>
       <c r="L165" s="2"/>
     </row>
-    <row r="166" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>226</v>
       </c>
@@ -12369,7 +12378,7 @@
       </c>
       <c r="L166" s="2"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>227</v>
       </c>
@@ -12405,7 +12414,7 @@
       </c>
       <c r="L167" s="2"/>
     </row>
-    <row r="168" spans="1:12" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4">
         <v>228</v>
       </c>
@@ -12441,7 +12450,7 @@
       </c>
       <c r="L168" s="9"/>
     </row>
-    <row r="169" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>229</v>
       </c>
@@ -12477,7 +12486,7 @@
       </c>
       <c r="L169" s="2"/>
     </row>
-    <row r="170" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>230</v>
       </c>
@@ -12513,7 +12522,7 @@
       </c>
       <c r="L170" s="2"/>
     </row>
-    <row r="171" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>231</v>
       </c>
@@ -12549,7 +12558,7 @@
       </c>
       <c r="L171" s="2"/>
     </row>
-    <row r="172" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>232</v>
       </c>
@@ -12585,7 +12594,7 @@
       </c>
       <c r="L172" s="2"/>
     </row>
-    <row r="173" spans="1:12" ht="30" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>233</v>
       </c>
@@ -12621,7 +12630,7 @@
       </c>
       <c r="L173" s="2"/>
     </row>
-    <row r="174" spans="1:12" ht="30" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>234</v>
       </c>
@@ -12657,7 +12666,7 @@
       </c>
       <c r="L174" s="2"/>
     </row>
-    <row r="175" spans="1:12" ht="30" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>235</v>
       </c>
@@ -12693,7 +12702,7 @@
       </c>
       <c r="L175" s="2"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>236</v>
       </c>
@@ -12729,7 +12738,7 @@
       </c>
       <c r="L176" s="2"/>
     </row>
-    <row r="177" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>237</v>
       </c>
@@ -12765,7 +12774,7 @@
       </c>
       <c r="L177" s="2"/>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>238</v>
       </c>
@@ -12801,7 +12810,7 @@
       </c>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>239</v>
       </c>
@@ -12837,7 +12846,7 @@
       </c>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>240</v>
       </c>
@@ -12876,7 +12885,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>241</v>
       </c>
@@ -12912,7 +12921,7 @@
       </c>
       <c r="L181" s="2"/>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>242</v>
       </c>
@@ -12948,7 +12957,7 @@
       </c>
       <c r="L182" s="2"/>
     </row>
-    <row r="183" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>243</v>
       </c>
@@ -12984,7 +12993,7 @@
       </c>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>244</v>
       </c>
@@ -13025,7 +13034,7 @@
       <c r="N184">
         <v>66.116667000000007</v>
       </c>
-      <c r="O184" s="30"/>
+      <c r="O184" s="26"/>
       <c r="P184" t="s">
         <v>727</v>
       </c>
@@ -13033,7 +13042,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>245</v>
       </c>
@@ -13069,7 +13078,7 @@
       </c>
       <c r="L185" s="2"/>
     </row>
-    <row r="186" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>246</v>
       </c>
@@ -13105,7 +13114,7 @@
       </c>
       <c r="L186" s="2"/>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>247</v>
       </c>
@@ -13141,7 +13150,7 @@
       </c>
       <c r="L187" s="2"/>
     </row>
-    <row r="188" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>248</v>
       </c>
@@ -13188,7 +13197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>249</v>
       </c>
@@ -13224,7 +13233,7 @@
       </c>
       <c r="L189" s="2"/>
     </row>
-    <row r="190" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>250</v>
       </c>
@@ -13260,7 +13269,7 @@
       </c>
       <c r="L190" s="2"/>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>251</v>
       </c>
@@ -13296,7 +13305,7 @@
       </c>
       <c r="L191" s="2"/>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>252</v>
       </c>
@@ -13332,7 +13341,7 @@
       </c>
       <c r="L192" s="2"/>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>253</v>
       </c>
@@ -13368,7 +13377,7 @@
       </c>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>254</v>
       </c>
@@ -13404,7 +13413,7 @@
       </c>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>255</v>
       </c>
@@ -13440,7 +13449,7 @@
       </c>
       <c r="L195" s="2"/>
     </row>
-    <row r="196" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="4">
         <v>256</v>
       </c>
@@ -13481,7 +13490,7 @@
       <c r="N196">
         <v>122.833333</v>
       </c>
-      <c r="O196" s="30"/>
+      <c r="O196" s="26"/>
       <c r="Q196">
         <v>1986</v>
       </c>
@@ -13492,7 +13501,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>257</v>
       </c>
@@ -13533,7 +13542,7 @@
       <c r="N197">
         <v>122.833333</v>
       </c>
-      <c r="O197" s="30"/>
+      <c r="O197" s="26"/>
       <c r="Q197">
         <v>1986</v>
       </c>
@@ -13544,7 +13553,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>258</v>
       </c>
@@ -13580,7 +13589,7 @@
       </c>
       <c r="L198" s="2"/>
     </row>
-    <row r="199" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>259</v>
       </c>
@@ -13616,7 +13625,7 @@
       </c>
       <c r="L199" s="2"/>
     </row>
-    <row r="200" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>260</v>
       </c>
@@ -13652,7 +13661,7 @@
       </c>
       <c r="L200" s="2"/>
     </row>
-    <row r="201" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>261</v>
       </c>
@@ -13688,7 +13697,7 @@
       </c>
       <c r="L201" s="2"/>
     </row>
-    <row r="202" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>262</v>
       </c>
@@ -13724,7 +13733,7 @@
       </c>
       <c r="L202" s="2"/>
     </row>
-    <row r="203" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A203" s="9">
         <v>263</v>
       </c>
@@ -13760,7 +13769,7 @@
       </c>
       <c r="L203" s="2"/>
     </row>
-    <row r="204" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>264</v>
       </c>
@@ -13801,7 +13810,7 @@
       <c r="N204">
         <v>-105.73653899999999</v>
       </c>
-      <c r="O204" s="30"/>
+      <c r="O204" s="26"/>
       <c r="P204" t="s">
         <v>711</v>
       </c>
@@ -13815,7 +13824,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>265</v>
       </c>
@@ -13856,7 +13865,7 @@
       <c r="N205">
         <v>-105.881742</v>
       </c>
-      <c r="O205" s="30"/>
+      <c r="O205" s="26"/>
       <c r="P205" t="s">
         <v>712</v>
       </c>
@@ -13870,7 +13879,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>266</v>
       </c>
@@ -13906,7 +13915,7 @@
       </c>
       <c r="L206" s="2"/>
     </row>
-    <row r="207" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A207" s="9">
         <v>267</v>
       </c>
@@ -13942,7 +13951,7 @@
       </c>
       <c r="L207" s="2"/>
     </row>
-    <row r="208" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>268</v>
       </c>
@@ -13978,7 +13987,7 @@
       </c>
       <c r="L208" s="2"/>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>269</v>
       </c>
@@ -14014,7 +14023,7 @@
       </c>
       <c r="L209" s="2"/>
     </row>
-    <row r="210" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>270</v>
       </c>
@@ -14050,7 +14059,7 @@
       </c>
       <c r="L210" s="2"/>
     </row>
-    <row r="211" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>271</v>
       </c>
@@ -14091,7 +14100,7 @@
       <c r="N211">
         <v>68.133332999999993</v>
       </c>
-      <c r="O211" s="30"/>
+      <c r="O211" s="26"/>
       <c r="P211" t="s">
         <v>729</v>
       </c>
@@ -14099,7 +14108,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>272</v>
       </c>
@@ -14135,7 +14144,7 @@
       </c>
       <c r="L212" s="2"/>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>273</v>
       </c>
@@ -14183,7 +14192,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>274</v>
       </c>
@@ -14228,7 +14237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>275</v>
       </c>
@@ -14276,7 +14285,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A216" s="9">
         <v>276</v>
       </c>
@@ -14324,7 +14333,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="40" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:19" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>277</v>
       </c>
@@ -14372,7 +14381,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>278</v>
       </c>
@@ -14421,7 +14430,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <v>279</v>
       </c>
@@ -14469,7 +14478,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>280</v>
       </c>
@@ -14517,7 +14526,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>281</v>
       </c>
@@ -14564,7 +14573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A222" s="9">
         <v>282</v>
       </c>
@@ -14611,7 +14620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>283</v>
       </c>
@@ -14652,7 +14661,7 @@
       <c r="N223">
         <v>65.150000000000006</v>
       </c>
-      <c r="O223" s="30"/>
+      <c r="O223" s="26"/>
       <c r="P223" t="s">
         <v>728</v>
       </c>
@@ -14660,7 +14669,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>284</v>
       </c>
@@ -14696,7 +14705,7 @@
       </c>
       <c r="L224" s="2"/>
     </row>
-    <row r="225" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>285</v>
       </c>
@@ -14732,7 +14741,7 @@
       </c>
       <c r="L225" s="2"/>
     </row>
-    <row r="226" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A226" s="4">
         <v>286</v>
       </c>
@@ -14768,7 +14777,7 @@
       </c>
       <c r="L226" s="2"/>
     </row>
-    <row r="227" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A227" s="6">
         <v>287</v>
       </c>
@@ -14804,7 +14813,7 @@
       </c>
       <c r="L227" s="2"/>
     </row>
-    <row r="228" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A228" s="9">
         <v>288</v>
       </c>
@@ -14840,7 +14849,7 @@
       </c>
       <c r="L228" s="2"/>
     </row>
-    <row r="229" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>289</v>
       </c>
@@ -14876,7 +14885,7 @@
       </c>
       <c r="L229" s="2"/>
     </row>
-    <row r="230" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <v>290</v>
       </c>
@@ -14912,7 +14921,7 @@
       </c>
       <c r="L230" s="2"/>
     </row>
-    <row r="231" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>291</v>
       </c>
@@ -14948,7 +14957,7 @@
       </c>
       <c r="L231" s="2"/>
     </row>
-    <row r="232" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A232" s="2">
         <v>292</v>
       </c>
@@ -14989,7 +14998,7 @@
       <c r="N232">
         <v>-106.830938</v>
       </c>
-      <c r="O232" s="30"/>
+      <c r="O232" s="26"/>
       <c r="Q232">
         <v>1919</v>
       </c>
@@ -15000,7 +15009,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>293</v>
       </c>
@@ -15036,7 +15045,7 @@
       </c>
       <c r="L233" s="2"/>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <v>294</v>
       </c>
@@ -15072,7 +15081,7 @@
       </c>
       <c r="L234" s="2"/>
     </row>
-    <row r="235" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>295</v>
       </c>
@@ -15108,7 +15117,7 @@
       </c>
       <c r="L235" s="2"/>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>296</v>
       </c>
@@ -15144,7 +15153,7 @@
       </c>
       <c r="L236" s="2"/>
     </row>
-    <row r="237" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>297</v>
       </c>
@@ -15180,7 +15189,7 @@
       </c>
       <c r="L237" s="2"/>
     </row>
-    <row r="238" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>298</v>
       </c>
@@ -15230,7 +15239,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <v>299</v>
       </c>
@@ -15266,7 +15275,7 @@
       </c>
       <c r="L239" s="2"/>
     </row>
-    <row r="240" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>300</v>
       </c>
@@ -15302,7 +15311,7 @@
       </c>
       <c r="L240" s="2"/>
     </row>
-    <row r="241" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <v>301</v>
       </c>
@@ -15338,7 +15347,7 @@
       </c>
       <c r="L241" s="2"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" s="2">
         <v>302</v>
       </c>
@@ -15374,7 +15383,7 @@
       </c>
       <c r="L242" s="2"/>
     </row>
-    <row r="243" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>303</v>
       </c>
@@ -15410,7 +15419,7 @@
       </c>
       <c r="L243" s="2"/>
     </row>
-    <row r="244" spans="1:12" ht="30" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>304</v>
       </c>
@@ -15446,7 +15455,7 @@
       </c>
       <c r="L244" s="2"/>
     </row>
-    <row r="245" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A245" s="2">
         <v>305</v>
       </c>
@@ -15482,7 +15491,7 @@
       </c>
       <c r="L245" s="2"/>
     </row>
-    <row r="246" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A246" s="2">
         <v>306</v>
       </c>
@@ -15518,7 +15527,7 @@
       </c>
       <c r="L246" s="2"/>
     </row>
-    <row r="247" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>307</v>
       </c>
@@ -15554,7 +15563,7 @@
       </c>
       <c r="L247" s="2"/>
     </row>
-    <row r="248" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A248" s="2">
         <v>308</v>
       </c>
@@ -15590,7 +15599,7 @@
       </c>
       <c r="L248" s="2"/>
     </row>
-    <row r="249" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>309</v>
       </c>
@@ -15626,7 +15635,7 @@
       </c>
       <c r="L249" s="2"/>
     </row>
-    <row r="250" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>310</v>
       </c>
@@ -15662,7 +15671,7 @@
       </c>
       <c r="L250" s="2"/>
     </row>
-    <row r="251" spans="1:12" ht="20" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>311</v>
       </c>
@@ -15698,7 +15707,7 @@
       </c>
       <c r="L251" s="2"/>
     </row>
-    <row r="252" spans="1:12" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A252" s="4">
         <v>312</v>
       </c>
@@ -15751,61 +15760,61 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" t="s">
         <v>525</v>
       </c>
@@ -15822,7 +15831,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>283</v>
       </c>
@@ -15869,7 +15878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>284</v>
       </c>
@@ -15916,7 +15925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>285</v>
       </c>
@@ -15963,7 +15972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>286</v>
       </c>
@@ -16010,7 +16019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>287</v>
       </c>
@@ -16057,7 +16066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>288</v>
       </c>
@@ -16104,7 +16113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>289</v>
       </c>
@@ -16151,7 +16160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>290</v>
       </c>
@@ -16198,7 +16207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>291</v>
       </c>
@@ -16245,7 +16254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>292</v>
       </c>
@@ -16292,7 +16301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>293</v>
       </c>
@@ -16339,7 +16348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>294</v>
       </c>
@@ -16392,7 +16401,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>295</v>
       </c>
@@ -16439,7 +16448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>296</v>
       </c>
@@ -16486,7 +16495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>297</v>
       </c>
@@ -16533,7 +16542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>298</v>
       </c>
@@ -16581,7 +16590,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>299</v>
       </c>
@@ -16631,7 +16640,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>300</v>
       </c>
@@ -16681,7 +16690,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>301</v>
       </c>
@@ -16731,7 +16740,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>304</v>
       </c>
@@ -16781,7 +16790,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>305</v>
       </c>
@@ -16828,7 +16837,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>306</v>
       </c>
@@ -16881,7 +16890,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>307</v>
       </c>
@@ -16931,7 +16940,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>308</v>
       </c>

</xml_diff>